<commit_message>
Checking out the changes
Checking out the changes in BugList file
</commit_message>
<xml_diff>
--- a/BugList/Требования. Баг Лист.xlsx
+++ b/BugList/Требования. Баг Лист.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei_Somov\Задание по лекциям\УЧЕБНЫЙ ПРОЕКТ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tatyana_Adnokulova@epam.com\Documents\GitHub\Project1\BugList\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Найденные дефекты" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Идентификатор</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Номер требования</t>
+  </si>
+  <si>
+    <t>Just checking it out. Tanya</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +482,9 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>

</xml_diff>